<commit_message>
modified:   WebRoot/page/agentcomp/addagent.jsp 	modified:   WebRoot/page/agentcomp/agentcomplist.jsp 	modified:   WebRoot/page/agentcomp/updagent.jsp 	modified:   WebRoot/page/audittempmetro.xlsx 	modified:   WebRoot/page/audittempnometro.xlsx 	modified:   WebRoot/page/info.jsp 	modified:   WebRoot/page/login.jsp 	modified:   src/com/cn/common/factory/PoiAuditMetro.java 	modified:   src/com/cn/tbps/action/BidProgressAction.java 	modified:   src/com/cn/tbps/dto/AgentCompDto.java 	modified:   src/com/cn/tbps/dto/AuditListDispEnum.java
</commit_message>
<xml_diff>
--- a/WebRoot/page/audittempmetro.xlsx
+++ b/WebRoot/page/audittempmetro.xlsx
@@ -15,8 +15,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">封面!$A$1:$F$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'审定单（地铁）'!$A$1:$U$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">签署页!$A$1:$H$34</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'审定单（地铁）'!$A$1:$U$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">资料登记表!$A$1:$I$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>项目预（结）算价审定单</t>
   </si>
@@ -591,11 +591,68 @@
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
   <si>
-    <t>（项目属性内的净核减额）</t>
+    <t>（生成表格日期）</t>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
   <si>
-    <t>（生成表格日期）</t>
+    <t>上海联合工程监理造价咨询有限公司</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海联合工程监理造价咨询有限公司会议室</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>（项</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目属性内的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>净</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>核减</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>额</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
 </sst>
@@ -611,7 +668,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -804,7 +861,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -816,7 +873,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -831,14 +888,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -850,6 +900,12 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1041,7 +1097,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1245,15 +1301,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1269,9 +1353,24 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1281,6 +1380,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1353,19 +1467,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1375,80 +1513,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="35" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1526,6 +1591,74 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>381087</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 5" descr="Logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7277100" y="5924550"/>
+          <a:ext cx="3095625" cy="257262"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1702,6 +1835,152 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1428750" cy="533400"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2838450" y="400050"/>
+          <a:ext cx="1428750" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 2" descr="Logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1571625" y="7972425"/>
+          <a:ext cx="3686175" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1998,7 +2277,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="R8" sqref="R8:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2007,29 +2286,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
     </row>
     <row r="2" spans="1:21" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="6"/>
@@ -2055,13 +2334,13 @@
       <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2082,165 +2361,165 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="128" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="130"/>
-      <c r="L4" s="131" t="s">
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="132" t="s">
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="132"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="132"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="132"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
     </row>
     <row r="5" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="133" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="135"/>
-      <c r="L5" s="131" t="s">
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
-      <c r="O5" s="136" t="s">
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="136"/>
-      <c r="Q5" s="136"/>
-      <c r="R5" s="136"/>
-      <c r="S5" s="136"/>
-      <c r="T5" s="136"/>
-      <c r="U5" s="136"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
     </row>
     <row r="6" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="136" t="s">
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="131"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="137" t="s">
-        <v>101</v>
-      </c>
-      <c r="P6" s="137"/>
-      <c r="Q6" s="137"/>
-      <c r="R6" s="137"/>
-      <c r="S6" s="137"/>
-      <c r="T6" s="137"/>
-      <c r="U6" s="137"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="92"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="92"/>
+      <c r="T6" s="92"/>
+      <c r="U6" s="92"/>
     </row>
     <row r="7" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="132" t="s">
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="132"/>
-      <c r="K7" s="138" t="s">
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="131" t="s">
+      <c r="L7" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="131"/>
-      <c r="N7" s="131"/>
-      <c r="O7" s="132" t="s">
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="P7" s="132"/>
-      <c r="Q7" s="132"/>
-      <c r="R7" s="132"/>
-      <c r="S7" s="132"/>
-      <c r="T7" s="132"/>
-      <c r="U7" s="138" t="s">
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="78" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="140" t="s">
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="131" t="s">
+      <c r="H8" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="140" t="s">
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="131" t="s">
+      <c r="O8" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="141" t="s">
-        <v>100</v>
-      </c>
-      <c r="S8" s="141"/>
-      <c r="T8" s="141"/>
-      <c r="U8" s="140" t="s">
+      <c r="P8" s="84"/>
+      <c r="Q8" s="84"/>
+      <c r="R8" s="85" t="s">
+        <v>103</v>
+      </c>
+      <c r="S8" s="144"/>
+      <c r="T8" s="144"/>
+      <c r="U8" s="79" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2291,33 +2570,33 @@
       <c r="U10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="82" t="s">
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="77" t="s">
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="99"/>
+      <c r="O11" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="78"/>
-      <c r="S11" s="78"/>
-      <c r="T11" s="78"/>
-      <c r="U11" s="79"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="88"/>
+      <c r="U11" s="89"/>
     </row>
     <row r="12" spans="1:21" ht="21.95" customHeight="1">
       <c r="A12" s="24"/>
@@ -2366,62 +2645,62 @@
       <c r="U13" s="28"/>
     </row>
     <row r="14" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="77" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="77" t="s">
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="78"/>
-      <c r="T14" s="78"/>
-      <c r="U14" s="79"/>
+      <c r="P14" s="88"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="88"/>
+      <c r="T14" s="88"/>
+      <c r="U14" s="89"/>
     </row>
     <row r="15" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="77" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="77" t="s">
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
-      <c r="T15" s="78"/>
-      <c r="U15" s="79"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="88"/>
+      <c r="S15" s="88"/>
+      <c r="T15" s="88"/>
+      <c r="U15" s="89"/>
     </row>
     <row r="16" spans="1:21" ht="21.95" customHeight="1">
       <c r="A16" s="13"/>
@@ -2474,8 +2753,8 @@
         <v>20</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2557,17 +2836,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
     </row>
     <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="30"/>
@@ -2585,13 +2864,13 @@
         <v>55</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="103" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="34"/>
       <c r="I3" s="35" t="s">
         <v>22</v>
@@ -2601,14 +2880,14 @@
       <c r="A4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
       <c r="H4" s="31" t="s">
         <v>25</v>
       </c>
@@ -2620,14 +2899,14 @@
       <c r="A5" s="32">
         <v>1</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
       <c r="H5" s="36"/>
       <c r="I5" s="32"/>
     </row>
@@ -2635,14 +2914,14 @@
       <c r="A6" s="32">
         <v>2</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
       <c r="H6" s="36"/>
       <c r="I6" s="32"/>
     </row>
@@ -2650,14 +2929,14 @@
       <c r="A7" s="32">
         <v>3</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
       <c r="H7" s="36"/>
       <c r="I7" s="32"/>
     </row>
@@ -2665,14 +2944,14 @@
       <c r="A8" s="32">
         <v>4</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
       <c r="H8" s="36"/>
       <c r="I8" s="32"/>
     </row>
@@ -2680,14 +2959,14 @@
       <c r="A9" s="32">
         <v>5</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
@@ -2695,14 +2974,14 @@
       <c r="A10" s="32">
         <v>6</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
       <c r="H10" s="36"/>
       <c r="I10" s="32"/>
     </row>
@@ -2710,14 +2989,14 @@
       <c r="A11" s="32">
         <v>7</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
       <c r="H11" s="36"/>
       <c r="I11" s="32"/>
     </row>
@@ -2725,14 +3004,14 @@
       <c r="A12" s="32">
         <v>8</v>
       </c>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
       <c r="H12" s="36"/>
       <c r="I12" s="32"/>
     </row>
@@ -2740,14 +3019,14 @@
       <c r="A13" s="32">
         <v>9</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
       <c r="H13" s="36"/>
       <c r="I13" s="32"/>
     </row>
@@ -2755,14 +3034,14 @@
       <c r="A14" s="32">
         <v>10</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
     </row>
@@ -2770,14 +3049,14 @@
       <c r="A15" s="32">
         <v>11</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
     </row>
@@ -2785,14 +3064,14 @@
       <c r="A16" s="32">
         <v>12</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
     </row>
@@ -2800,14 +3079,14 @@
       <c r="A17" s="32">
         <v>13</v>
       </c>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
     </row>
@@ -2815,14 +3094,14 @@
       <c r="A18" s="32">
         <v>14</v>
       </c>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
       <c r="H18" s="36"/>
       <c r="I18" s="32"/>
     </row>
@@ -2830,14 +3109,14 @@
       <c r="A19" s="32">
         <v>15</v>
       </c>
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="105"/>
       <c r="H19" s="36"/>
       <c r="I19" s="32"/>
     </row>
@@ -2845,14 +3124,14 @@
       <c r="A20" s="32">
         <v>16</v>
       </c>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
       <c r="H20" s="36"/>
       <c r="I20" s="32"/>
     </row>
@@ -2860,14 +3139,14 @@
       <c r="A21" s="32">
         <v>17</v>
       </c>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
     </row>
@@ -2875,158 +3154,158 @@
       <c r="A22" s="32">
         <v>18</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="85"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
-      <c r="A23" s="87"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="89"/>
+      <c r="A23" s="107"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="109"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="90" t="s">
+      <c r="B24" s="111"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="110" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="91"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="90" t="s">
+      <c r="E24" s="111"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="110" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="91"/>
-      <c r="I24" s="92"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="112"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="91"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="90" t="s">
+      <c r="B25" s="111"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="91"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="90" t="s">
+      <c r="E25" s="111"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="91"/>
-      <c r="I25" s="92"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="112"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1">
-      <c r="A26" s="94"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="96"/>
+      <c r="A26" s="114"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="116"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1">
-      <c r="A27" s="90" t="s">
+      <c r="A27" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="90" t="s">
+      <c r="B27" s="111"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="91"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="90" t="s">
+      <c r="E27" s="111"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="91"/>
-      <c r="I27" s="92"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="112"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1">
-      <c r="A28" s="100"/>
-      <c r="B28" s="101"/>
-      <c r="C28" s="102"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="102"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="102"/>
+      <c r="A28" s="120"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="120"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="122"/>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="91"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="90" t="s">
+      <c r="B29" s="111"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="91"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="90" t="s">
+      <c r="E29" s="111"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="91"/>
-      <c r="I29" s="92"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="112"/>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="94"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="96"/>
+      <c r="A30" s="114"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="114"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="116"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="97" t="s">
+      <c r="A31" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="98"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="97" t="s">
+      <c r="B31" s="118"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="98"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="97" t="s">
+      <c r="E31" s="118"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="98"/>
-      <c r="I31" s="99"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="119"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="104"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="104"/>
-      <c r="F32" s="104"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="105"/>
+      <c r="B32" s="124"/>
+      <c r="C32" s="124"/>
+      <c r="D32" s="124"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -3095,7 +3374,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3104,15 +3383,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="41"/>
@@ -3131,32 +3410,34 @@
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="F3" s="111" t="s">
+      <c r="F3" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="111"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="135" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
     </row>
     <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
+      <c r="B5" s="137" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
       <c r="F5" s="40" t="s">
         <v>60</v>
       </c>
@@ -3166,16 +3447,18 @@
       <c r="A6" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="73" t="s">
         <v>87</v>
       </c>
       <c r="C6" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="D6" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="139"/>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1">
       <c r="A7" s="44"/>
@@ -3370,71 +3653,73 @@
       <c r="A28" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="106"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106" t="s">
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
     </row>
     <row r="29" spans="1:7" ht="35.1" customHeight="1">
       <c r="A29" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="121" t="s">
+      <c r="B29" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="122"/>
-      <c r="D29" s="122"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
     </row>
     <row r="30" spans="1:7" ht="35.1" customHeight="1">
       <c r="A30" s="40"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="122"/>
-      <c r="D30" s="122"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="126"/>
+      <c r="F30" s="126"/>
+      <c r="G30" s="126"/>
     </row>
     <row r="31" spans="1:7" ht="35.1" customHeight="1">
       <c r="A31" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="121" t="s">
+      <c r="B31" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="122"/>
-      <c r="D31" s="122"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126"/>
     </row>
     <row r="32" spans="1:7" ht="35.1" customHeight="1">
       <c r="A32" s="40"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="126"/>
     </row>
     <row r="33" spans="1:7" ht="35.1" customHeight="1">
       <c r="A33" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="107"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="106"/>
+      <c r="B33" s="129" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="127"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="126"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="38"/>
@@ -3446,24 +3731,24 @@
       <c r="G34" s="38"/>
     </row>
     <row r="35" spans="1:7" ht="14.25">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="110"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="133"/>
     </row>
     <row r="36" spans="1:7" ht="14.25">
-      <c r="A36" s="108"/>
-      <c r="B36" s="108"/>
-      <c r="C36" s="108"/>
-      <c r="D36" s="108"/>
-      <c r="E36" s="108"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="108"/>
+      <c r="A36" s="128"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3503,7 +3788,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3528,28 +3813,28 @@
       <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="141" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
       <c r="F3" s="53"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
       <c r="F4" s="53"/>
     </row>
     <row r="5" spans="2:6" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
       <c r="F5" s="58"/>
     </row>
     <row r="6" spans="2:6" ht="18.75" thickTop="1">
@@ -3563,7 +3848,7 @@
       <c r="C7" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="124" t="s">
+      <c r="D7" s="74" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="53"/>
@@ -3572,7 +3857,7 @@
       <c r="C8" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="75" t="s">
         <v>95</v>
       </c>
       <c r="F8" s="53"/>
@@ -3689,7 +3974,7 @@
   <dimension ref="B1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3710,14 +3995,14 @@
       <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:8" ht="60" customHeight="1">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
       <c r="H2" s="61"/>
     </row>
     <row r="3" spans="2:8" ht="17.100000000000001" customHeight="1">
@@ -3733,7 +4018,7 @@
       <c r="B4" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="76" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="61"/>
@@ -3746,7 +4031,7 @@
       <c r="B5" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="77" t="s">
         <v>79</v>
       </c>
       <c r="D5" s="61"/>
@@ -3959,14 +4244,14 @@
     </row>
     <row r="34" spans="2:8" ht="17.25">
       <c r="B34" s="61"/>
-      <c r="C34" s="114" t="s">
+      <c r="C34" s="142" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="114"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="142"/>
     </row>
     <row r="36" spans="2:8" ht="14.25">
       <c r="B36" s="70"/>
@@ -3985,5 +4270,6 @@
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   WebRoot/page/audit/addaudit.jsp 	modified:   WebRoot/page/audit/auditlist.jsp 	modified:   WebRoot/page/audit/updaudit.jsp 	modified:   WebRoot/page/audittempmetro.xlsx 	modified:   WebRoot/page/audittempnometro.xlsx
</commit_message>
<xml_diff>
--- a/WebRoot/page/audittempmetro.xlsx
+++ b/WebRoot/page/audittempmetro.xlsx
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>填表人：</t>
-  </si>
-  <si>
-    <t>审价资料提供情况登记表</t>
   </si>
   <si>
     <t>SUECC/OI01-T-0705F</t>
@@ -441,10 +438,6 @@
     <t>注：本纪要一式　　份，参加会议单位各执一份。</t>
   </si>
   <si>
-    <t>会商纪要</t>
-    <phoneticPr fontId="32" type="noConversion"/>
-  </si>
-  <si>
     <t>结算审核报告</t>
   </si>
   <si>
@@ -479,9 +472,6 @@
       </rPr>
       <t/>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">           证书编号：甲150331000541</t>
   </si>
   <si>
     <t>（项目属性内的项目文号）</t>
@@ -653,6 +643,18 @@
       </rPr>
       <t>）</t>
     </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>审价资料提供情况登记表</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>会商纪要</t>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">           证书编号：甲190331000541</t>
     <phoneticPr fontId="32" type="noConversion"/>
   </si>
 </sst>
@@ -1097,7 +1099,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1320,74 +1322,134 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="30" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1396,71 +1458,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1469,36 +1498,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1513,8 +1512,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="36" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1669,6 +1674,89 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>511175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 2" descr="Logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="28575" y="57150"/>
+          <a:ext cx="3775075" cy="454025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -1767,10 +1855,88 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>511175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 2" descr="Logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="57150" y="57150"/>
+          <a:ext cx="4645025" cy="454025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1901,7 +2067,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2286,29 +2452,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
     </row>
     <row r="2" spans="1:21" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="6"/>
@@ -2334,13 +2500,13 @@
       <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="35.1" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2366,30 +2532,30 @@
       </c>
       <c r="B4" s="83"/>
       <c r="C4" s="83"/>
-      <c r="D4" s="100" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="84" t="s">
+      <c r="D4" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
     </row>
     <row r="5" spans="1:21" ht="35.1" customHeight="1">
       <c r="A5" s="83" t="s">
@@ -2397,30 +2563,30 @@
       </c>
       <c r="B5" s="83"/>
       <c r="C5" s="83"/>
-      <c r="D5" s="94" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="84" t="s">
+      <c r="D5" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="91" t="s">
-        <v>97</v>
-      </c>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
-      <c r="U5" s="91"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="99"/>
+      <c r="U5" s="99"/>
     </row>
     <row r="6" spans="1:21" ht="35.1" customHeight="1">
       <c r="A6" s="83" t="s">
@@ -2428,28 +2594,28 @@
       </c>
       <c r="B6" s="83"/>
       <c r="C6" s="83"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="91" t="s">
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="92" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="92"/>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
     </row>
     <row r="7" spans="1:21" ht="35.1" customHeight="1">
       <c r="A7" s="83" t="s">
@@ -2457,31 +2623,31 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
-      <c r="D7" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
+      <c r="D7" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="82"/>
-      <c r="T7" s="82"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
       <c r="U7" s="78" t="s">
         <v>10</v>
       </c>
@@ -2492,33 +2658,33 @@
       </c>
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="84" t="s">
+      <c r="H8" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="95"/>
       <c r="N8" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="84" t="s">
+      <c r="O8" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="S8" s="144"/>
-      <c r="T8" s="144"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8" s="96"/>
+      <c r="T8" s="96"/>
       <c r="U8" s="79" t="s">
         <v>10</v>
       </c>
@@ -2570,33 +2736,33 @@
       <c r="U10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="97" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="87" t="s">
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="88"/>
-      <c r="S11" s="88"/>
-      <c r="T11" s="88"/>
-      <c r="U11" s="89"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="82"/>
     </row>
     <row r="12" spans="1:21" ht="21.95" customHeight="1">
       <c r="A12" s="24"/>
@@ -2645,62 +2811,62 @@
       <c r="U13" s="28"/>
     </row>
     <row r="14" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="87" t="s">
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="87" t="s">
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="88"/>
-      <c r="R14" s="88"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="89"/>
+      <c r="P14" s="81"/>
+      <c r="Q14" s="81"/>
+      <c r="R14" s="81"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="82"/>
     </row>
     <row r="15" spans="1:21" ht="21.95" customHeight="1">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="87" t="s">
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="87" t="s">
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="88"/>
-      <c r="U15" s="89"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81"/>
+      <c r="R15" s="81"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="82"/>
     </row>
     <row r="16" spans="1:21" ht="21.95" customHeight="1">
       <c r="A16" s="13"/>
@@ -2753,8 +2919,8 @@
         <v>20</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2775,18 +2941,13 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="O15:U15"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="O11:U11"/>
-    <mergeCell ref="O14:U14"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="K8:M8"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="H15:N15"/>
@@ -2803,13 +2964,18 @@
     <mergeCell ref="D6:K6"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="O15:U15"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="O11:U11"/>
+    <mergeCell ref="O14:U14"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="D4:K4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2827,7 +2993,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2835,20 +3001,20 @@
     <col min="8" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="113" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="66.75" customHeight="1">
+      <c r="A1" s="143" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1">
       <c r="A2" s="30"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2861,52 +3027,52 @@
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="103" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
+      <c r="C3" s="123" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
       <c r="H3" s="34"/>
       <c r="I3" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1">
       <c r="A4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="31" t="s">
+      <c r="I4" s="31" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="24.95" customHeight="1">
       <c r="A5" s="32">
         <v>1</v>
       </c>
-      <c r="B5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
+      <c r="B5" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
       <c r="H5" s="36"/>
       <c r="I5" s="32"/>
     </row>
@@ -2914,14 +3080,14 @@
       <c r="A6" s="32">
         <v>2</v>
       </c>
-      <c r="B6" s="105" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
+      <c r="B6" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
       <c r="H6" s="36"/>
       <c r="I6" s="32"/>
     </row>
@@ -2929,14 +3095,14 @@
       <c r="A7" s="32">
         <v>3</v>
       </c>
-      <c r="B7" s="105" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
+      <c r="B7" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
       <c r="H7" s="36"/>
       <c r="I7" s="32"/>
     </row>
@@ -2944,14 +3110,14 @@
       <c r="A8" s="32">
         <v>4</v>
       </c>
-      <c r="B8" s="105" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
+      <c r="B8" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
       <c r="H8" s="36"/>
       <c r="I8" s="32"/>
     </row>
@@ -2959,14 +3125,14 @@
       <c r="A9" s="32">
         <v>5</v>
       </c>
-      <c r="B9" s="105" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
+      <c r="B9" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="119"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
@@ -2974,14 +3140,14 @@
       <c r="A10" s="32">
         <v>6</v>
       </c>
-      <c r="B10" s="105" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
+      <c r="B10" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
       <c r="H10" s="36"/>
       <c r="I10" s="32"/>
     </row>
@@ -2989,14 +3155,14 @@
       <c r="A11" s="32">
         <v>7</v>
       </c>
-      <c r="B11" s="105" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
+      <c r="B11" s="119" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="119"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
       <c r="H11" s="36"/>
       <c r="I11" s="32"/>
     </row>
@@ -3004,14 +3170,14 @@
       <c r="A12" s="32">
         <v>8</v>
       </c>
-      <c r="B12" s="105" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
+      <c r="B12" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
       <c r="H12" s="36"/>
       <c r="I12" s="32"/>
     </row>
@@ -3019,14 +3185,14 @@
       <c r="A13" s="32">
         <v>9</v>
       </c>
-      <c r="B13" s="105" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
+      <c r="B13" s="119" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="119"/>
       <c r="H13" s="36"/>
       <c r="I13" s="32"/>
     </row>
@@ -3034,14 +3200,14 @@
       <c r="A14" s="32">
         <v>10</v>
       </c>
-      <c r="B14" s="105" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
+      <c r="B14" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="119"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
     </row>
@@ -3049,14 +3215,14 @@
       <c r="A15" s="32">
         <v>11</v>
       </c>
-      <c r="B15" s="105" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
+      <c r="B15" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
     </row>
@@ -3064,14 +3230,14 @@
       <c r="A16" s="32">
         <v>12</v>
       </c>
-      <c r="B16" s="105" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
+      <c r="B16" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
     </row>
@@ -3079,14 +3245,14 @@
       <c r="A17" s="32">
         <v>13</v>
       </c>
-      <c r="B17" s="105" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
+      <c r="B17" s="119" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
     </row>
@@ -3094,14 +3260,14 @@
       <c r="A18" s="32">
         <v>14</v>
       </c>
-      <c r="B18" s="105" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
+      <c r="B18" s="119" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
       <c r="H18" s="36"/>
       <c r="I18" s="32"/>
     </row>
@@ -3109,14 +3275,14 @@
       <c r="A19" s="32">
         <v>15</v>
       </c>
-      <c r="B19" s="105" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
+      <c r="B19" s="119" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="119"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="119"/>
       <c r="H19" s="36"/>
       <c r="I19" s="32"/>
     </row>
@@ -3124,14 +3290,14 @@
       <c r="A20" s="32">
         <v>16</v>
       </c>
-      <c r="B20" s="105" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
+      <c r="B20" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
       <c r="H20" s="36"/>
       <c r="I20" s="32"/>
     </row>
@@ -3139,14 +3305,14 @@
       <c r="A21" s="32">
         <v>17</v>
       </c>
-      <c r="B21" s="105" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
+      <c r="B21" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="119"/>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
     </row>
@@ -3154,168 +3320,187 @@
       <c r="A22" s="32">
         <v>18</v>
       </c>
-      <c r="B22" s="105" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
+      <c r="B22" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
-      <c r="A23" s="107"/>
-      <c r="B23" s="108"/>
-      <c r="C23" s="109"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="109"/>
+      <c r="A23" s="120"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="122"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="A24" s="110" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="110" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="111"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="110" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="111"/>
-      <c r="I24" s="112"/>
+      <c r="A24" s="107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="108"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="107" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="108"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="107" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="108"/>
+      <c r="I24" s="109"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="108"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="108"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="108"/>
+      <c r="I25" s="109"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1">
+      <c r="A26" s="113"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="115"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="114"/>
+      <c r="I26" s="115"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" customHeight="1">
+      <c r="A27" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="110" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="111"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="110" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="111"/>
-      <c r="I25" s="112"/>
-    </row>
-    <row r="26" spans="1:9" ht="18" customHeight="1">
-      <c r="A26" s="114"/>
-      <c r="B26" s="115"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="114"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="116"/>
-    </row>
-    <row r="27" spans="1:9" ht="18" customHeight="1">
-      <c r="A27" s="110" t="s">
+      <c r="B27" s="108"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="110" t="s">
+      <c r="E27" s="108"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="111"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="110" t="s">
+      <c r="H27" s="108"/>
+      <c r="I27" s="109"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" customHeight="1">
+      <c r="A28" s="110"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="112"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" customHeight="1">
+      <c r="A29" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="111"/>
-      <c r="I27" s="112"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1">
-      <c r="A28" s="120"/>
-      <c r="B28" s="121"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="120"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="122"/>
-    </row>
-    <row r="29" spans="1:9" ht="18" customHeight="1">
-      <c r="A29" s="110" t="s">
+      <c r="B29" s="108"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="108"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="110" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="111"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="110" t="s">
+      <c r="H29" s="108"/>
+      <c r="I29" s="109"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1">
+      <c r="A30" s="113"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="115"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="114"/>
+      <c r="F30" s="115"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="115"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1">
+      <c r="A31" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="111"/>
-      <c r="I29" s="112"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="114"/>
-      <c r="B30" s="115"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="116"/>
-    </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="117" t="s">
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="118"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="117" t="s">
+      <c r="E31" s="117"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="118"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="117" t="s">
+      <c r="H31" s="117"/>
+      <c r="I31" s="118"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1">
+      <c r="A32" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="118"/>
-      <c r="I31" s="119"/>
-    </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1">
-      <c r="A32" s="123" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="124"/>
-      <c r="C32" s="124"/>
-      <c r="D32" s="124"/>
-      <c r="E32" s="124"/>
-      <c r="F32" s="124"/>
-      <c r="G32" s="124"/>
-      <c r="H32" s="124"/>
-      <c r="I32" s="125"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
@@ -3332,37 +3517,19 @@
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D31:F31"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3371,10 +3538,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3382,18 +3549,25 @@
     <col min="1" max="7" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1">
-      <c r="A1" s="130" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:14" ht="60.75" customHeight="1">
+      <c r="A1" s="144" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+    </row>
+    <row r="2" spans="1:14" ht="23.25" customHeight="1">
       <c r="A2" s="41"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -3402,65 +3576,65 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="3" spans="1:7" ht="24.95" customHeight="1">
+    <row r="3" spans="1:14" ht="24.95" customHeight="1">
       <c r="A3" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="130" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="130"/>
+    </row>
+    <row r="4" spans="1:14" ht="39.950000000000003" customHeight="1">
+      <c r="A4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="134"/>
-    </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="B4" s="131" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+    </row>
+    <row r="5" spans="1:14" ht="39.950000000000003" customHeight="1">
+      <c r="A5" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="135" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-    </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A5" s="40" t="s">
+      <c r="B5" s="133" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="137" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="40" t="s">
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="1:14" ht="39.950000000000003" customHeight="1">
+      <c r="A6" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A6" s="43" t="s">
+      <c r="B6" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="138" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-    </row>
-    <row r="7" spans="1:7" ht="24.95" customHeight="1">
+      <c r="D6" s="134" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+    </row>
+    <row r="7" spans="1:14" ht="24.95" customHeight="1">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
@@ -3469,7 +3643,7 @@
       <c r="F7" s="45"/>
       <c r="G7" s="46"/>
     </row>
-    <row r="8" spans="1:7" ht="24.95" customHeight="1">
+    <row r="8" spans="1:14" ht="24.95" customHeight="1">
       <c r="A8" s="47"/>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
@@ -3478,7 +3652,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="48"/>
     </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1">
+    <row r="9" spans="1:14" ht="24.95" customHeight="1">
       <c r="A9" s="47"/>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -3487,7 +3661,7 @@
       <c r="F9" s="42"/>
       <c r="G9" s="48"/>
     </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1">
+    <row r="10" spans="1:14" ht="24.95" customHeight="1">
       <c r="A10" s="47"/>
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
@@ -3496,7 +3670,7 @@
       <c r="F10" s="42"/>
       <c r="G10" s="48"/>
     </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1">
+    <row r="11" spans="1:14" ht="24.95" customHeight="1">
       <c r="A11" s="47"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -3505,7 +3679,7 @@
       <c r="F11" s="42"/>
       <c r="G11" s="48"/>
     </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1">
+    <row r="12" spans="1:14" ht="24.95" customHeight="1">
       <c r="A12" s="47"/>
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
@@ -3514,7 +3688,7 @@
       <c r="F12" s="42"/>
       <c r="G12" s="48"/>
     </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1">
+    <row r="13" spans="1:14" ht="24.95" customHeight="1">
       <c r="A13" s="47"/>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
@@ -3523,7 +3697,7 @@
       <c r="F13" s="42"/>
       <c r="G13" s="48"/>
     </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1">
+    <row r="14" spans="1:14" ht="24.95" customHeight="1">
       <c r="A14" s="47"/>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -3532,7 +3706,7 @@
       <c r="F14" s="42"/>
       <c r="G14" s="48"/>
     </row>
-    <row r="15" spans="1:7" ht="24.95" customHeight="1">
+    <row r="15" spans="1:14" ht="24.95" customHeight="1">
       <c r="A15" s="47"/>
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
@@ -3541,7 +3715,7 @@
       <c r="F15" s="42"/>
       <c r="G15" s="48"/>
     </row>
-    <row r="16" spans="1:7" ht="24.95" customHeight="1">
+    <row r="16" spans="1:14" ht="24.95" customHeight="1">
       <c r="A16" s="47"/>
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
@@ -3651,75 +3825,75 @@
     </row>
     <row r="28" spans="1:7" ht="35.1" customHeight="1">
       <c r="A28" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="126" t="s">
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
+      <c r="E28" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="126" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="128"/>
     </row>
     <row r="29" spans="1:7" ht="35.1" customHeight="1">
       <c r="A29" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="131" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="132"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="126"/>
+        <v>85</v>
+      </c>
+      <c r="B29" s="126" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="128"/>
+      <c r="G29" s="128"/>
     </row>
     <row r="30" spans="1:7" ht="35.1" customHeight="1">
       <c r="A30" s="40"/>
-      <c r="B30" s="132"/>
-      <c r="C30" s="132"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="126"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="126"/>
+      <c r="B30" s="127"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="128"/>
+      <c r="F30" s="128"/>
+      <c r="G30" s="128"/>
     </row>
     <row r="31" spans="1:7" ht="35.1" customHeight="1">
       <c r="A31" s="72" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="131" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="132"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="126"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="126"/>
+        <v>86</v>
+      </c>
+      <c r="B31" s="126" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="127"/>
+      <c r="D31" s="127"/>
+      <c r="E31" s="128"/>
+      <c r="F31" s="128"/>
+      <c r="G31" s="128"/>
     </row>
     <row r="32" spans="1:7" ht="35.1" customHeight="1">
       <c r="A32" s="40"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="126"/>
+      <c r="B32" s="136"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
     </row>
     <row r="33" spans="1:7" ht="35.1" customHeight="1">
       <c r="A33" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="129" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="127"/>
-      <c r="D33" s="127"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="126"/>
-      <c r="G33" s="126"/>
+        <v>65</v>
+      </c>
+      <c r="B33" s="138" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="136"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="38"/>
@@ -3731,27 +3905,30 @@
       <c r="G34" s="38"/>
     </row>
     <row r="35" spans="1:7" ht="14.25">
-      <c r="A35" s="133" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="133"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="133"/>
-      <c r="G35" s="133"/>
+      <c r="A35" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="129"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="129"/>
     </row>
     <row r="36" spans="1:7" ht="14.25">
-      <c r="A36" s="128"/>
-      <c r="B36" s="128"/>
-      <c r="C36" s="128"/>
-      <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
-      <c r="G36" s="128"/>
+      <c r="A36" s="137"/>
+      <c r="B36" s="137"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="E29:G29"/>
@@ -3768,9 +3945,6 @@
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3813,28 +3987,28 @@
       <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B3" s="141" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
+      <c r="B3" s="140" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="53"/>
     </row>
     <row r="4" spans="2:6" ht="50.1" customHeight="1">
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="53"/>
     </row>
     <row r="5" spans="2:6" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B5" s="140" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
+      <c r="B5" s="139" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="58"/>
     </row>
     <row r="6" spans="2:6" ht="18.75" thickTop="1">
@@ -3846,19 +4020,19 @@
     </row>
     <row r="7" spans="2:6" ht="24.95" customHeight="1">
       <c r="C7" s="60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F7" s="53"/>
     </row>
     <row r="8" spans="2:6" ht="24.95" customHeight="1">
       <c r="C8" s="60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F8" s="53"/>
     </row>
@@ -3974,7 +4148,7 @@
   <dimension ref="B1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3995,14 +4169,14 @@
       <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:8" ht="60" customHeight="1">
-      <c r="B2" s="143" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
+      <c r="B2" s="142" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
       <c r="H2" s="61"/>
     </row>
     <row r="3" spans="2:8" ht="17.100000000000001" customHeight="1">
@@ -4016,10 +4190,10 @@
     </row>
     <row r="4" spans="2:8" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="61"/>
       <c r="E4" s="61"/>
@@ -4029,10 +4203,10 @@
     </row>
     <row r="5" spans="2:8" ht="17.100000000000001" customHeight="1">
       <c r="B5" s="67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
@@ -4051,7 +4225,7 @@
     </row>
     <row r="7" spans="2:8" ht="35.1" customHeight="1">
       <c r="B7" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
@@ -4107,11 +4281,11 @@
     </row>
     <row r="13" spans="2:8" ht="17.25">
       <c r="B13" s="68" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="71"/>
       <c r="D13" s="68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13" s="61"/>
       <c r="F13" s="61"/>
@@ -4157,11 +4331,11 @@
     </row>
     <row r="19" spans="2:4" ht="17.25">
       <c r="B19" s="68" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="71"/>
       <c r="D19" s="68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="17.25">
@@ -4191,11 +4365,11 @@
     </row>
     <row r="25" spans="2:4" ht="17.25">
       <c r="B25" s="68" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="68" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="17.25">
@@ -4244,14 +4418,14 @@
     </row>
     <row r="34" spans="2:8" ht="17.25">
       <c r="B34" s="61"/>
-      <c r="C34" s="142" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="142"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="142"/>
+      <c r="C34" s="141" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="141"/>
+      <c r="G34" s="141"/>
+      <c r="H34" s="141"/>
     </row>
     <row r="36" spans="2:8" ht="14.25">
       <c r="B36" s="70"/>

</xml_diff>